<commit_message>
api to return data csv
</commit_message>
<xml_diff>
--- a/psrivastava48_individual_Gantt_Chart.xlsx
+++ b/psrivastava48_individual_Gantt_Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F7CDB5-E551-254B-A9CE-81BF1A6C6F78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612652A6-4530-BD46-892C-CE6F4571D2FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19240" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23560" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t>Members</t>
   </si>
   <si>
-    <t>Individual Project: Drug Abuse</t>
-  </si>
-  <si>
     <t>Week # 11</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                                         </t>
+  </si>
+  <si>
+    <t>Individual Project: Drug Abuse Prevention</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -713,6 +712,7 @@
     <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1230,7 +1230,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
@@ -1284,136 +1284,136 @@
       <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="57">
+      <c r="H4" s="56">
         <f>H5</f>
         <v>44137</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="57">
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="56">
         <f>O5</f>
         <v>44144</v>
       </c>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="57">
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="56">
         <f>V5</f>
         <v>44151</v>
       </c>
-      <c r="W4" s="58"/>
-      <c r="X4" s="58"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="58"/>
-      <c r="AB4" s="59"/>
-      <c r="AC4" s="57">
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="57"/>
+      <c r="Z4" s="57"/>
+      <c r="AA4" s="57"/>
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="56">
         <f>AC5</f>
         <v>44158</v>
       </c>
-      <c r="AD4" s="58"/>
-      <c r="AE4" s="58"/>
-      <c r="AF4" s="58"/>
-      <c r="AG4" s="58"/>
-      <c r="AH4" s="58"/>
-      <c r="AI4" s="59"/>
-      <c r="AJ4" s="57">
+      <c r="AD4" s="57"/>
+      <c r="AE4" s="57"/>
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="57"/>
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="58"/>
+      <c r="AJ4" s="56">
         <f>AJ5</f>
         <v>44165</v>
       </c>
-      <c r="AK4" s="58"/>
-      <c r="AL4" s="58"/>
-      <c r="AM4" s="58"/>
-      <c r="AN4" s="58"/>
-      <c r="AO4" s="58"/>
-      <c r="AP4" s="59"/>
-      <c r="AQ4" s="57">
+      <c r="AK4" s="57"/>
+      <c r="AL4" s="57"/>
+      <c r="AM4" s="57"/>
+      <c r="AN4" s="57"/>
+      <c r="AO4" s="57"/>
+      <c r="AP4" s="58"/>
+      <c r="AQ4" s="56">
         <f>AQ5</f>
         <v>44172</v>
       </c>
-      <c r="AR4" s="58"/>
-      <c r="AS4" s="58"/>
-      <c r="AT4" s="58"/>
-      <c r="AU4" s="58"/>
-      <c r="AV4" s="58"/>
-      <c r="AW4" s="59"/>
-      <c r="AX4" s="57">
+      <c r="AR4" s="57"/>
+      <c r="AS4" s="57"/>
+      <c r="AT4" s="57"/>
+      <c r="AU4" s="57"/>
+      <c r="AV4" s="57"/>
+      <c r="AW4" s="58"/>
+      <c r="AX4" s="56">
         <f>AX5</f>
         <v>44179</v>
       </c>
-      <c r="AY4" s="58"/>
-      <c r="AZ4" s="58"/>
-      <c r="BA4" s="58"/>
-      <c r="BB4" s="58"/>
-      <c r="BC4" s="58"/>
-      <c r="BD4" s="59"/>
-      <c r="BE4" s="57">
+      <c r="AY4" s="57"/>
+      <c r="AZ4" s="57"/>
+      <c r="BA4" s="57"/>
+      <c r="BB4" s="57"/>
+      <c r="BC4" s="57"/>
+      <c r="BD4" s="58"/>
+      <c r="BE4" s="56">
         <f>BE5</f>
         <v>44186</v>
       </c>
-      <c r="BF4" s="58"/>
-      <c r="BG4" s="58"/>
-      <c r="BH4" s="58"/>
-      <c r="BI4" s="58"/>
-      <c r="BJ4" s="58"/>
-      <c r="BK4" s="59"/>
-      <c r="BL4" s="57">
+      <c r="BF4" s="57"/>
+      <c r="BG4" s="57"/>
+      <c r="BH4" s="57"/>
+      <c r="BI4" s="57"/>
+      <c r="BJ4" s="57"/>
+      <c r="BK4" s="58"/>
+      <c r="BL4" s="56">
         <f>BL5</f>
         <v>44193</v>
       </c>
-      <c r="BM4" s="58"/>
-      <c r="BN4" s="58"/>
-      <c r="BO4" s="58"/>
-      <c r="BP4" s="58"/>
-      <c r="BQ4" s="58"/>
-      <c r="BR4" s="59"/>
-      <c r="BS4" s="57">
+      <c r="BM4" s="57"/>
+      <c r="BN4" s="57"/>
+      <c r="BO4" s="57"/>
+      <c r="BP4" s="57"/>
+      <c r="BQ4" s="57"/>
+      <c r="BR4" s="58"/>
+      <c r="BS4" s="56">
         <f>BS5</f>
         <v>44200</v>
       </c>
-      <c r="BT4" s="58"/>
-      <c r="BU4" s="58"/>
-      <c r="BV4" s="58"/>
-      <c r="BW4" s="58"/>
-      <c r="BX4" s="58"/>
-      <c r="BY4" s="59"/>
-      <c r="BZ4" s="57">
+      <c r="BT4" s="57"/>
+      <c r="BU4" s="57"/>
+      <c r="BV4" s="57"/>
+      <c r="BW4" s="57"/>
+      <c r="BX4" s="57"/>
+      <c r="BY4" s="58"/>
+      <c r="BZ4" s="56">
         <f>BZ5</f>
         <v>44207</v>
       </c>
-      <c r="CA4" s="58"/>
-      <c r="CB4" s="58"/>
-      <c r="CC4" s="58"/>
-      <c r="CD4" s="58"/>
-      <c r="CE4" s="58"/>
-      <c r="CF4" s="59"/>
-      <c r="CG4" s="57">
+      <c r="CA4" s="57"/>
+      <c r="CB4" s="57"/>
+      <c r="CC4" s="57"/>
+      <c r="CD4" s="57"/>
+      <c r="CE4" s="57"/>
+      <c r="CF4" s="58"/>
+      <c r="CG4" s="56">
         <f>CG5</f>
         <v>44214</v>
       </c>
-      <c r="CH4" s="58"/>
-      <c r="CI4" s="58"/>
-      <c r="CJ4" s="58"/>
-      <c r="CK4" s="58"/>
-      <c r="CL4" s="58"/>
-      <c r="CM4" s="59"/>
+      <c r="CH4" s="57"/>
+      <c r="CI4" s="57"/>
+      <c r="CJ4" s="57"/>
+      <c r="CK4" s="57"/>
+      <c r="CL4" s="57"/>
+      <c r="CM4" s="58"/>
     </row>
     <row r="5" spans="1:91" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
       <c r="H5" s="9">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44137</v>
@@ -2207,7 +2207,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -2307,7 +2307,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="18">
         <v>1</v>
@@ -2415,7 +2415,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="18">
         <v>1</v>
@@ -2521,7 +2521,7 @@
     <row r="11" spans="1:91" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
       <c r="B11" s="48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="18">
         <v>1</v>
@@ -2629,10 +2629,10 @@
         <v>21</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
@@ -2729,7 +2729,7 @@
     <row r="13" spans="1:91" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="23">
         <v>1</v>
@@ -2835,7 +2835,7 @@
     <row r="14" spans="1:91" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="23">
         <v>1</v>
@@ -2943,7 +2943,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="26"/>
@@ -3041,7 +3041,7 @@
     <row r="16" spans="1:91" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37"/>
       <c r="B16" s="50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="28">
         <v>1</v>
@@ -3147,7 +3147,7 @@
     <row r="17" spans="1:91" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="28">
         <v>1</v>
@@ -3252,7 +3252,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="31"/>
@@ -3350,7 +3350,7 @@
     <row r="19" spans="1:91" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="33">
         <v>1</v>
@@ -3456,10 +3456,10 @@
     <row r="20" spans="1:91" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37"/>
       <c r="B20" s="51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="45">
         <f>E17+1</f>
@@ -3562,10 +3562,10 @@
     <row r="21" spans="1:91" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="45">
         <f>E17+1</f>
@@ -3667,17 +3667,11 @@
     </row>
     <row r="23" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="BL4:BR4"/>
-    <mergeCell ref="BS4:BY4"/>
-    <mergeCell ref="BZ4:CF4"/>
-    <mergeCell ref="CG4:CM4"/>
-    <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="BE4:BK4"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AQ4:AW4"/>
@@ -3686,6 +3680,12 @@
     <mergeCell ref="O4:U4"/>
     <mergeCell ref="V4:AB4"/>
     <mergeCell ref="AC4:AI4"/>
+    <mergeCell ref="BL4:BR4"/>
+    <mergeCell ref="BS4:BY4"/>
+    <mergeCell ref="BZ4:CF4"/>
+    <mergeCell ref="CG4:CM4"/>
+    <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="BE4:BK4"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C13 C15:C21">
     <cfRule type="dataBar" priority="31">
@@ -3735,7 +3735,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="43" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -3836,33 +3836,11 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="ac51c468-00e1-45df-a915-d2c818df2c1a">
-      <UserInfo>
-        <DisplayName>Bhattacharjee, Arunabh</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010052304ACAA711F54A869B529C597CD26E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="165981f183fd3fa19277ca051bb432e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6518d7dd-6f7c-48eb-9716-9ee25839745a" xmlns:ns3="ac51c468-00e1-45df-a915-d2c818df2c1a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddbf9f4d50cd9781bff302a32a2c3de4" ns2:_="" ns3:_="">
     <xsd:import namespace="6518d7dd-6f7c-48eb-9716-9ee25839745a"/>
@@ -4067,10 +4045,44 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="ac51c468-00e1-45df-a915-d2c818df2c1a">
+      <UserInfo>
+        <DisplayName>Bhattacharjee, Arunabh</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{206335CA-C17D-4325-BC71-B55B6F9852F7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{340D1667-27E4-4276-A931-8841D804D76E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6518d7dd-6f7c-48eb-9716-9ee25839745a"/>
+    <ds:schemaRef ds:uri="ac51c468-00e1-45df-a915-d2c818df2c1a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4093,20 +4105,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{340D1667-27E4-4276-A931-8841D804D76E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{206335CA-C17D-4325-BC71-B55B6F9852F7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6518d7dd-6f7c-48eb-9716-9ee25839745a"/>
-    <ds:schemaRef ds:uri="ac51c468-00e1-45df-a915-d2c818df2c1a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>